<commit_message>
Término das correções solicitadas pela Eunice
</commit_message>
<xml_diff>
--- a/docs/projeto-final/pfc/apendices/APÊNDICE B - PRODUCT BACKLOG E SPRINTS/PRODUCT BACKLOG E SPRINTS.xlsx
+++ b/docs/projeto-final/pfc/apendices/APÊNDICE B - PRODUCT BACKLOG E SPRINTS/PRODUCT BACKLOG E SPRINTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusjbarbosa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusjbarbosa/Desktop/Desenvolvimento/repositorios/fai/fai.etanois.docs/docs/projeto-final/pfc/apendices/APÊNDICE B - PRODUCT BACKLOG E SPRINTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79BB5B9D-1BDF-F143-8C5A-AB487D8A11DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DFA098-BCCE-9640-A660-82EF501B416D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="28240" windowHeight="17560" activeTab="2" xr2:uid="{27DFC456-3B12-044F-B229-CAFE82F2B1CD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{27DFC456-3B12-044F-B229-CAFE82F2B1CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
   <si>
     <t>etanóis - Product Backlog</t>
   </si>
@@ -152,6 +152,21 @@
   </si>
   <si>
     <t>etanóis - Sprint II</t>
+  </si>
+  <si>
+    <t>Início</t>
+  </si>
+  <si>
+    <t>Fim</t>
+  </si>
+  <si>
+    <t>PRIORIDADE</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Alta</t>
   </si>
 </sst>
 </file>
@@ -204,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -216,6 +231,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -532,311 +550,420 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F107A857-5273-D347-B67F-4ED286D796F5}">
-  <dimension ref="B2:C38"/>
+  <dimension ref="B2:D38"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="C42" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="5.83203125" style="3"/>
     <col min="3" max="3" width="77.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="5.83203125" style="3"/>
+    <col min="4" max="4" width="16.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="5.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="60" customHeight="1">
+    <row r="2" spans="2:4" ht="60" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="2:3" ht="35" customHeight="1">
+    <row r="3" spans="2:4" ht="35" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="20" customHeight="1">
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="20" customHeight="1">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="20" customHeight="1">
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="20" customHeight="1">
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="20" customHeight="1">
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="20" customHeight="1">
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="20" customHeight="1">
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="20" customHeight="1">
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="20" customHeight="1">
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="20" customHeight="1">
       <c r="B8" s="3">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="20" customHeight="1">
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="20" customHeight="1">
       <c r="B9" s="3">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="20" customHeight="1">
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="20" customHeight="1">
       <c r="B10" s="3">
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" ht="20" customHeight="1">
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="20" customHeight="1">
       <c r="B11" s="3">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="20" customHeight="1">
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20" customHeight="1">
       <c r="B12" s="3">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="20" customHeight="1">
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" customHeight="1">
       <c r="B13" s="3">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="20" customHeight="1">
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="20" customHeight="1">
       <c r="B14" s="3">
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="20" customHeight="1">
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="20" customHeight="1">
       <c r="B15" s="3">
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="20" customHeight="1">
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="20" customHeight="1">
       <c r="B16" s="3">
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="20" customHeight="1">
+      <c r="D16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="20" customHeight="1">
       <c r="B17" s="3">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="20" customHeight="1">
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="20" customHeight="1">
       <c r="B18" s="3">
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="20" customHeight="1">
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="20" customHeight="1">
       <c r="B19" s="3">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="20" customHeight="1">
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="20" customHeight="1">
       <c r="B20" s="3">
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="20" customHeight="1">
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="20" customHeight="1">
       <c r="B21" s="3">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" ht="20" customHeight="1">
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="20" customHeight="1">
       <c r="B22" s="3">
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" ht="20" customHeight="1">
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="20" customHeight="1">
       <c r="B23" s="3">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" ht="20" customHeight="1">
+      <c r="D23" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" customHeight="1">
       <c r="B24" s="3">
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" ht="20" customHeight="1">
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="20" customHeight="1">
       <c r="B25" s="3">
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" ht="20" customHeight="1">
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="20" customHeight="1">
       <c r="B26" s="3">
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" ht="20" customHeight="1">
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="20" customHeight="1">
       <c r="B27" s="3">
         <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" ht="20" customHeight="1">
+      <c r="D27" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="20" customHeight="1">
       <c r="B28" s="3">
         <v>25</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" ht="20" customHeight="1">
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="20" customHeight="1">
       <c r="B29" s="3">
         <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" ht="20" customHeight="1">
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="20" customHeight="1">
       <c r="B30" s="3">
         <v>27</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" ht="20" customHeight="1">
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="20" customHeight="1">
       <c r="B31" s="3">
         <v>28</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" ht="20" customHeight="1">
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="20" customHeight="1">
       <c r="B32" s="3">
         <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" ht="20" customHeight="1">
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="20" customHeight="1">
       <c r="B33" s="3">
         <v>30</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" ht="20" customHeight="1">
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="20" customHeight="1">
       <c r="B34" s="3">
         <v>31</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" ht="20" customHeight="1">
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="20" customHeight="1">
       <c r="B35" s="3">
         <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" ht="20" customHeight="1">
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="20" customHeight="1">
       <c r="B36" s="3">
         <v>33</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" ht="20" customHeight="1">
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="20" customHeight="1">
       <c r="B37" s="3">
         <v>34</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" ht="20" customHeight="1">
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="20" customHeight="1">
       <c r="B38" s="3">
         <v>35</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>36</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -849,42 +976,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8699DB-32B6-6443-B57B-FCF56E3101E9}">
-  <dimension ref="B2:C17"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="5.83203125" style="3"/>
     <col min="3" max="3" width="77.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="5.83203125" style="3"/>
+    <col min="4" max="4" width="5.83203125" style="3"/>
+    <col min="5" max="5" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="5.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="60" customHeight="1">
+    <row r="2" spans="2:6" ht="60" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="2:3" ht="35" customHeight="1">
+    <row r="3" spans="2:6" ht="35" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="20" customHeight="1">
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="20" customHeight="1">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="20" customHeight="1">
+      <c r="E4" s="5">
+        <v>43891</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43918</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="20" customHeight="1">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -892,7 +1034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="20" customHeight="1">
+    <row r="6" spans="2:6" ht="20" customHeight="1">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -900,7 +1042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20" customHeight="1">
+    <row r="7" spans="2:6" ht="20" customHeight="1">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -908,7 +1050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="20" customHeight="1">
+    <row r="8" spans="2:6" ht="20" customHeight="1">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -916,7 +1058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="20" customHeight="1">
+    <row r="9" spans="2:6" ht="20" customHeight="1">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -924,7 +1066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="20" customHeight="1">
+    <row r="10" spans="2:6" ht="20" customHeight="1">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -932,7 +1074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="20" customHeight="1">
+    <row r="11" spans="2:6" ht="20" customHeight="1">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -940,7 +1082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="20" customHeight="1">
+    <row r="12" spans="2:6" ht="20" customHeight="1">
       <c r="B12" s="3">
         <v>9</v>
       </c>
@@ -948,7 +1090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="20" customHeight="1">
+    <row r="13" spans="2:6" ht="20" customHeight="1">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -956,7 +1098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="20" customHeight="1">
+    <row r="14" spans="2:6" ht="20" customHeight="1">
       <c r="B14" s="3">
         <v>11</v>
       </c>
@@ -964,7 +1106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="20" customHeight="1">
+    <row r="15" spans="2:6" ht="20" customHeight="1">
       <c r="B15" s="3">
         <v>12</v>
       </c>
@@ -972,7 +1114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="20" customHeight="1">
+    <row r="16" spans="2:6" ht="20" customHeight="1">
       <c r="B16" s="3">
         <v>13</v>
       </c>
@@ -995,42 +1137,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620735E5-C44E-3444-8966-74434372C19E}">
-  <dimension ref="B2:C24"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="5.83203125" style="3"/>
     <col min="3" max="3" width="77.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="5.83203125" style="3"/>
+    <col min="4" max="4" width="5.83203125" style="3"/>
+    <col min="5" max="6" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="5.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="60" customHeight="1">
+    <row r="2" spans="2:6" ht="60" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="2:3" ht="35" customHeight="1">
+    <row r="3" spans="2:6" ht="35" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="20" customHeight="1">
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="20" customHeight="1">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="20" customHeight="1">
+      <c r="E4" s="5">
+        <v>43920</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43974</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="20" customHeight="1">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1038,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="20" customHeight="1">
+    <row r="6" spans="2:6" ht="20" customHeight="1">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1046,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20" customHeight="1">
+    <row r="7" spans="2:6" ht="20" customHeight="1">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -1054,7 +1210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="20" customHeight="1">
+    <row r="8" spans="2:6" ht="20" customHeight="1">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -1062,7 +1218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="20" customHeight="1">
+    <row r="9" spans="2:6" ht="20" customHeight="1">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -1070,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="20" customHeight="1">
+    <row r="10" spans="2:6" ht="20" customHeight="1">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -1078,7 +1234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="20" customHeight="1">
+    <row r="11" spans="2:6" ht="20" customHeight="1">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -1086,7 +1242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="20" customHeight="1">
+    <row r="12" spans="2:6" ht="20" customHeight="1">
       <c r="B12" s="3">
         <v>9</v>
       </c>
@@ -1094,7 +1250,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="20" customHeight="1">
+    <row r="13" spans="2:6" ht="20" customHeight="1">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -1102,7 +1258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="20" customHeight="1">
+    <row r="14" spans="2:6" ht="20" customHeight="1">
       <c r="B14" s="3">
         <v>11</v>
       </c>
@@ -1110,7 +1266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="20" customHeight="1">
+    <row r="15" spans="2:6" ht="20" customHeight="1">
       <c r="B15" s="3">
         <v>12</v>
       </c>
@@ -1118,7 +1274,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="20" customHeight="1">
+    <row r="16" spans="2:6" ht="20" customHeight="1">
       <c r="B16" s="3">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Atualização das sprints e backlog
</commit_message>
<xml_diff>
--- a/docs/projeto-final/pfc/apendices/APÊNDICE B - PRODUCT BACKLOG E SPRINTS/PRODUCT BACKLOG E SPRINTS.xlsx
+++ b/docs/projeto-final/pfc/apendices/APÊNDICE B - PRODUCT BACKLOG E SPRINTS/PRODUCT BACKLOG E SPRINTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusjbarbosa/Documents/Desenvolvimento/Repos/fai.etanois.docs/docs/projeto-final/pfc/apendices/APÊNDICE B - PRODUCT BACKLOG E SPRINTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BB5CD8-4AFA-7947-9BF5-E5E7BE7174BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D400FD0-BC8B-9B41-85B1-47F1A24E5F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{27DFC456-3B12-044F-B229-CAFE82F2B1CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="51">
   <si>
     <t>etanóis - Product Backlog</t>
   </si>
@@ -195,7 +195,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +220,17 @@
       <color theme="1"/>
       <name val="Poppins Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Poppins Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Poppins Regular"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -255,17 +266,23 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,549 +600,549 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F107A857-5273-D347-B67F-4ED286D796F5}">
   <dimension ref="B2:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="5.83203125" style="7"/>
-    <col min="3" max="3" width="77.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="5.83203125" style="7"/>
+    <col min="1" max="2" width="5.83203125" style="5"/>
+    <col min="3" max="3" width="77.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="5.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="60" customHeight="1">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="2:4" ht="35" customHeight="1">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="20" customHeight="1">
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="20" customHeight="1">
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="20" customHeight="1">
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" customHeight="1">
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20" customHeight="1">
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" customHeight="1">
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" customHeight="1">
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="20" customHeight="1">
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="20" customHeight="1">
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" customHeight="1">
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" customHeight="1">
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="20" customHeight="1">
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="20" customHeight="1">
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="20" customHeight="1">
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20" customHeight="1">
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="20" customHeight="1">
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>16</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="20" customHeight="1">
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>17</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="20" customHeight="1">
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="20" customHeight="1">
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="20" customHeight="1">
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="20" customHeight="1">
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>21</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="20" customHeight="1">
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>22</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="20" customHeight="1">
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>23</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="20" customHeight="1">
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>24</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="20" customHeight="1">
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>25</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20" customHeight="1">
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>26</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="20" customHeight="1">
-      <c r="B30" s="7">
+      <c r="B30" s="5">
         <v>27</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20" customHeight="1">
-      <c r="B31" s="7">
+      <c r="B31" s="5">
         <v>28</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20" customHeight="1">
-      <c r="B32" s="7">
+      <c r="B32" s="5">
         <v>29</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20" customHeight="1">
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <v>30</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="20" customHeight="1">
-      <c r="B34" s="7">
+      <c r="B34" s="5">
         <v>31</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="20" customHeight="1">
-      <c r="B35" s="7">
+      <c r="B35" s="5">
         <v>32</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="20" customHeight="1">
-      <c r="B36" s="7">
+      <c r="B36" s="5">
         <v>33</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="20" customHeight="1">
-      <c r="B37" s="7">
+      <c r="B37" s="5">
         <v>34</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="20" customHeight="1">
-      <c r="B38" s="7">
+      <c r="B38" s="5">
         <v>35</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="39" customHeight="1">
-      <c r="B39" s="7">
+      <c r="B39" s="5">
         <v>36</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="39" customHeight="1">
-      <c r="B40" s="7">
+      <c r="B40" s="5">
         <v>37</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="39" customHeight="1">
-      <c r="B41" s="7">
+      <c r="B41" s="5">
         <v>38</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="39" customHeight="1">
-      <c r="B42" s="7">
+      <c r="B42" s="5">
         <v>39</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="44" customHeight="1">
-      <c r="B43" s="7">
+      <c r="B43" s="5">
         <v>40</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="44" customHeight="1">
-      <c r="B44" s="7">
+      <c r="B44" s="5">
         <v>41</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="44" customHeight="1">
-      <c r="B45" s="7">
+      <c r="B45" s="5">
         <v>42</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="44" customHeight="1">
-      <c r="B46" s="7">
-        <v>43</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="B46" s="5">
+        <v>43</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="44" customHeight="1">
-      <c r="B47" s="7">
+      <c r="B47" s="5">
         <v>44</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="44" customHeight="1">
-      <c r="B48" s="7">
+      <c r="B48" s="5">
         <v>45</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="44" customHeight="1">
-      <c r="B49" s="7">
+      <c r="B49" s="5">
         <v>46</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="44" customHeight="1">
-      <c r="B50" s="7">
+      <c r="B50" s="5">
         <v>47</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1143,14 +1160,14 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D3" sqref="D3:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="5.83203125" style="3"/>
     <col min="3" max="3" width="77.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="3"/>
+    <col min="4" max="4" width="26" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="5.83203125" style="3"/>
@@ -1169,6 +1186,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1183,6 +1203,9 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E4" s="4">
         <v>43891</v>
       </c>
@@ -1197,6 +1220,9 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="20" customHeight="1">
       <c r="B6" s="3">
@@ -1205,6 +1231,9 @@
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="20" customHeight="1">
       <c r="B7" s="3">
@@ -1213,6 +1242,9 @@
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="20" customHeight="1">
       <c r="B8" s="3">
@@ -1221,6 +1253,9 @@
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="20" customHeight="1">
       <c r="B9" s="3">
@@ -1229,6 +1264,9 @@
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="2:6" ht="20" customHeight="1">
       <c r="B10" s="3">
@@ -1237,6 +1275,9 @@
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="2:6" ht="20" customHeight="1">
       <c r="B11" s="3">
@@ -1245,6 +1286,9 @@
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="2:6" ht="20" customHeight="1">
       <c r="B12" s="3">
@@ -1253,6 +1297,9 @@
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="2:6" ht="20" customHeight="1">
       <c r="B13" s="3">
@@ -1261,6 +1308,9 @@
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="2:6" ht="20" customHeight="1">
       <c r="B14" s="3">
@@ -1269,6 +1319,9 @@
       <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="2:6" ht="20" customHeight="1">
       <c r="B15" s="3">
@@ -1277,6 +1330,9 @@
       <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="2:6" ht="20" customHeight="1">
       <c r="B16" s="3">
@@ -1285,13 +1341,19 @@
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="20" customHeight="1">
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="20" customHeight="1">
       <c r="B17" s="3">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1304,23 +1366,23 @@
   <dimension ref="B2:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:XFD1048576"/>
+      <selection activeCell="D3" sqref="D3:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="5.83203125" style="3"/>
     <col min="3" max="3" width="77.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="3"/>
+    <col min="4" max="4" width="32.1640625" style="3" customWidth="1"/>
     <col min="5" max="6" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="5.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="60" customHeight="1">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="2:6" ht="35" customHeight="1">
       <c r="B3" s="2" t="s">
@@ -1329,6 +1391,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1343,6 +1408,9 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="4">
         <v>43920</v>
       </c>
@@ -1357,6 +1425,9 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="20" customHeight="1">
       <c r="B6" s="3">
@@ -1365,6 +1436,9 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="20" customHeight="1">
       <c r="B7" s="3">
@@ -1373,6 +1447,9 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="20" customHeight="1">
       <c r="B8" s="3">
@@ -1381,6 +1458,9 @@
       <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="20" customHeight="1">
       <c r="B9" s="3">
@@ -1389,6 +1469,9 @@
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="2:6" ht="20" customHeight="1">
       <c r="B10" s="3">
@@ -1397,6 +1480,9 @@
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="2:6" ht="20" customHeight="1">
       <c r="B11" s="3">
@@ -1405,6 +1491,9 @@
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="2:6" ht="20" customHeight="1">
       <c r="B12" s="3">
@@ -1413,6 +1502,9 @@
       <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="2:6" ht="20" customHeight="1">
       <c r="B13" s="3">
@@ -1421,6 +1513,9 @@
       <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="2:6" ht="20" customHeight="1">
       <c r="B14" s="3">
@@ -1429,6 +1524,9 @@
       <c r="C14" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="2:6" ht="20" customHeight="1">
       <c r="B15" s="3">
@@ -1437,6 +1535,9 @@
       <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="2:6" ht="20" customHeight="1">
       <c r="B16" s="3">
@@ -1445,69 +1546,96 @@
       <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="20" customHeight="1">
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="20" customHeight="1">
       <c r="B17" s="3">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="20" customHeight="1">
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="20" customHeight="1">
       <c r="B18" s="3">
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="20" customHeight="1">
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="20" customHeight="1">
       <c r="B19" s="3">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="20" customHeight="1">
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="20" customHeight="1">
       <c r="B20" s="3">
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="20" customHeight="1">
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="20" customHeight="1">
       <c r="B21" s="3">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" ht="20" customHeight="1">
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="20" customHeight="1">
       <c r="B22" s="3">
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" ht="20" customHeight="1">
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="20" customHeight="1">
       <c r="B23" s="3">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" ht="20" customHeight="1">
+      <c r="D23" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" customHeight="1">
       <c r="B24" s="3">
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>36</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1520,26 +1648,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098D9EDA-CF27-2249-A286-5A3028705A54}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="5.83203125" style="3"/>
     <col min="3" max="3" width="77.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="3"/>
+    <col min="4" max="4" width="32.1640625" style="3" customWidth="1"/>
     <col min="5" max="6" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="5.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="60" customHeight="1">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="2:6" ht="35" customHeight="1">
       <c r="B3" s="2" t="s">
@@ -1548,6 +1676,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1559,8 +1690,11 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="E4" s="4">
         <v>43974</v>
@@ -1573,92 +1707,144 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="44" customHeight="1">
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="44" customHeight="1">
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="44" customHeight="1">
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="44" customHeight="1">
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="44" customHeight="1">
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="44" customHeight="1">
       <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="44" customHeight="1">
       <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>48</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="44" customHeight="1">
       <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="44" customHeight="1">
       <c r="B14" s="3">
         <v>11</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="44" customHeight="1">
       <c r="B15" s="3">
         <v>12</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="D15" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="2:6" ht="20" customHeight="1">
-      <c r="C16" s="7"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="4:4" ht="20" customHeight="1">
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="4:4" ht="20" customHeight="1">
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="4:4" ht="20" customHeight="1">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="4:4" ht="20" customHeight="1">
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="4:4" ht="20" customHeight="1">
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="4:4" ht="20" customHeight="1">
+      <c r="D22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>